<commit_message>
ADDED BARCODE TO CALL SHEETS
</commit_message>
<xml_diff>
--- a/ARCHIVE/deployment/Omaha_Cal_Info_CP02PMCI_00007.xlsx
+++ b/ARCHIVE/deployment/Omaha_Cal_Info_CP02PMCI_00007.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtravis\Documents\Vault\Project_Files\Documentation\Coastal_Pioneer\Coastal Pioneer Notebook\Pioneer 7 Deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leila/Documents/OOI_assmgt/asset-management/ARCHIVE/deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3084" yWindow="1500" windowWidth="9156" windowHeight="3348" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="29580" yWindow="-2920" windowWidth="19640" windowHeight="13680" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,20 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$B$1:$K$76</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$H$405</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="67">
   <si>
     <t>Ref Des</t>
   </si>
@@ -201,9 +209,6 @@
     <t>43-2499</t>
   </si>
   <si>
-    <t>12991-02</t>
-  </si>
-  <si>
     <t>SWE 0008 Rev G</t>
   </si>
   <si>
@@ -214,12 +219,42 @@
   </si>
   <si>
     <t>AR-08</t>
+  </si>
+  <si>
+    <t>A00491</t>
+  </si>
+  <si>
+    <t>N00037</t>
+  </si>
+  <si>
+    <t>N00036</t>
+  </si>
+  <si>
+    <t>N00041</t>
+  </si>
+  <si>
+    <t>N00038</t>
+  </si>
+  <si>
+    <t>A00286.1</t>
+  </si>
+  <si>
+    <t>OL000239</t>
+  </si>
+  <si>
+    <t>ML12991-02</t>
+  </si>
+  <si>
+    <t>RS00001</t>
+  </si>
+  <si>
+    <t>RM00002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -401,7 +436,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -464,30 +499,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -509,42 +546,57 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="0" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="76">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -575,6 +627,13 @@
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -605,6 +664,13 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Asset_Cal_Info" xfId="55"/>
   </cellStyles>
@@ -735,9 +801,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -770,9 +836,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -979,93 +1045,95 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="7" width="15.77734375" customWidth="1"/>
-    <col min="8" max="9" width="19.77734375" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" customWidth="1"/>
-    <col min="12" max="12" width="26.77734375" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="9" width="19.83203125" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" customWidth="1"/>
     <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:14" ht="28" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="12" t="s">
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7">
+        <v>7</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="13">
-        <v>7</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1075,842 +1143,983 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
-    <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="12" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="47" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="5">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="26">
+      <c r="B2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="15">
+        <v>7</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="17">
         <v>20495</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="22"/>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="5">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="26">
+      <c r="B3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="15">
+        <v>7</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="17">
         <v>20495</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="H3" s="20"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="5">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="26">
+      <c r="B4" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="15">
+        <v>7</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="17">
         <v>20495</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="H4" s="20"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="5">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E7" s="2"/>
-      <c r="F7" s="25"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="15">
+        <v>7</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E7" s="16"/>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="5">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="26" t="s">
+      <c r="B8" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="15">
+        <v>7</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="23">
         <v>-850.28</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="5">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="26" t="s">
+      <c r="B9" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="15">
+        <v>7</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="H9" s="20"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="5">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="26" t="s">
+      <c r="B10" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="15">
+        <v>7</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="H10" s="20"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="5">
-        <v>7</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="26" t="s">
+      <c r="B11" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="15">
+        <v>7</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="23">
         <v>3.1894999999999997E-4</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="5">
-        <v>7</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="26" t="s">
+      <c r="B12" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="15">
+        <v>7</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="23">
         <v>-3.0959E-3</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="5">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="26" t="s">
+      <c r="B13" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="15">
+        <v>7</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="23">
         <v>1.6605999999999999E-4</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="5">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="26" t="s">
+      <c r="B14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="15">
+        <v>7</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="23">
         <v>-2.6610999999999998E-6</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="5">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="26" t="s">
+      <c r="B15" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="15">
+        <v>7</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="23">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="5">
-        <v>7</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="26">
+      <c r="B17" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="15">
+        <v>7</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="17">
         <v>113</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="21"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="H17" s="20"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="5">
-        <v>7</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="26">
+      <c r="B18" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="15">
+        <v>7</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="17">
         <v>113</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="H18" s="20"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="5">
-        <v>7</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="26">
+      <c r="B20" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="15">
+        <v>7</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="17">
         <v>100013</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="H20" s="20"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="5">
-        <v>7</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="26">
+      <c r="B21" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="15">
+        <v>7</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="17">
         <v>100013</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="21"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="H21" s="20"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="5">
-        <v>7</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="26">
+      <c r="B23" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="15">
+        <v>7</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="17">
         <v>1031</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="25">
         <v>1.0760000000000001</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="J23" s="18"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="5">
-        <v>7</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="26">
+      <c r="B24" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="15">
+        <v>7</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="17">
         <v>1031</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="26">
         <v>47</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="I24" s="15"/>
+      <c r="J24" s="18"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="5">
-        <v>7</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="26">
+      <c r="B25" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="15">
+        <v>7</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="17">
         <v>1031</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="26">
         <v>46</v>
       </c>
-      <c r="I25" s="5"/>
-      <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="I25" s="15"/>
+      <c r="J25" s="18"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="5">
-        <v>7</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="26">
+      <c r="B26" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="15">
+        <v>7</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="17">
         <v>1031</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H26" s="26">
         <v>49</v>
       </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="5">
-        <v>7</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="26">
+      <c r="B27" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="15">
+        <v>7</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="17">
         <v>1031</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="27">
         <v>3.9E-2</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="5">
-        <v>7</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="26">
+      <c r="B28" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="15">
+        <v>7</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="17">
         <v>1031</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="27">
         <v>700</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="5">
-        <v>7</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="26">
+      <c r="B29" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="15">
+        <v>7</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="17">
         <v>1031</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H29" s="18">
+      <c r="H29" s="26">
         <v>7.2300000000000003E-2</v>
       </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="I29" s="28"/>
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="5">
-        <v>7</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="26">
+      <c r="B30" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="15">
+        <v>7</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="17">
         <v>1031</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H30" s="26">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="5">
-        <v>7</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="26">
+      <c r="B31" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="15">
+        <v>7</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="17">
         <v>1031</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="18">
+      <c r="H31" s="26">
         <v>3.1540000000000002E-6</v>
       </c>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="5">
-        <v>7</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="26">
+      <c r="B32" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="15">
+        <v>7</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="17">
         <v>1031</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="H32" s="24">
+      <c r="H32" s="27">
         <v>124</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="I32" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="J32" s="18"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="5">
-        <v>7</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="26">
+      <c r="B34" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="15">
+        <v>7</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="17">
         <v>20447</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H34" s="18">
+      <c r="H34" s="26">
         <v>1</v>
       </c>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="5">
-        <v>7</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="26">
+      <c r="B35" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="15">
+        <v>7</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="17">
         <v>20447</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H35" s="30">
+      <c r="H35" s="26">
         <v>9.9199999999999996E-18</v>
       </c>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="5">
-        <v>7</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="25" t="s">
+      <c r="B37" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="15">
+        <v>7</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E38" s="16"/>
+      <c r="F38" s="22"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="15">
+        <v>7</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E38" s="2"/>
-      <c r="F38" s="25"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="5">
-        <v>7</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F40" s="19"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F42" s="7"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F43" s="7"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E40" s="16"/>
+      <c r="F40" s="30"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E41" s="16"/>
+      <c r="F41" s="31"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E42" s="16"/>
+      <c r="F42" s="31"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E43" s="16"/>
+      <c r="F43" s="31"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E44" s="16"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E45" s="16"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E46" s="16"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E47" s="16"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E48" s="16"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E49" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>